<commit_message>
updated yaml to remove version
</commit_message>
<xml_diff>
--- a/process/configuration/templates/generate_policy_report_options.xlsx
+++ b/process/configuration/templates/generate_policy_report_options.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27813"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="8_{5371514D-1DBE-4717-AFC4-8A4C5449F29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC1CF2EE-2AAF-4682-8534-AA372D0417A4}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{5371514D-1DBE-4717-AFC4-8A4C5449F29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9D3D0C7-9EC1-4CDD-B4E6-732007D31ED8}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A0E12F1D-6A69-4722-9AF0-AE48B14A4F0D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{A0E12F1D-6A69-4722-9AF0-AE48B14A4F0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Language options" sheetId="1" r:id="rId1"/>
     <sheet name="General options" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,69 +39,165 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="67">
   <si>
+    <t>Global Observatory of Healthy and Sustainable Cities</t>
+  </si>
+  <si>
     <t>Policy report configuration options</t>
   </si>
   <si>
+    <t>Version 0.01</t>
+  </si>
+  <si>
+    <t>21 June 2024</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Additional language* (rename this cell)</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>City name, for example: مَسْقَط</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Country name, for example: سلطنة عُمان</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>After reviewing the results, update this summary text to contextualise your findings, and relate to external text and documents (e.g. using website hyperlinks).  This text will be used in the report summary.</t>
+  </si>
+  <si>
+    <t>City context</t>
+  </si>
+  <si>
+    <t>Please briefly summarise the city location, history and topography, as relevant.</t>
+  </si>
+  <si>
+    <t>Demographics and health equity</t>
+  </si>
+  <si>
+    <t>Please highlight socio-economic demographic characteristics and key health challenges and inequities present in this urban area.</t>
+  </si>
+  <si>
+    <t>Environmental disaster context:</t>
+  </si>
+  <si>
+    <t>Completed policy checklist values will be added, but prose may be customised here to detail  environmental hazards likely to be experience by the urban area over the next 5-10 years</t>
+  </si>
+  <si>
+    <t>Levels of Government</t>
+  </si>
+  <si>
+    <t>Completed policy checklist values will be added, but prose may be customised here to detail levels of government reviewed in the policy checklist using the appropriate terms for your study region.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Pending validation, additional language options may include: </t>
+  </si>
+  <si>
+    <t>Arabic</t>
+  </si>
+  <si>
+    <t>Catalan</t>
+  </si>
+  <si>
+    <t>Chinese - Simplified</t>
+  </si>
+  <si>
+    <t>Chinese - Traditional</t>
+  </si>
+  <si>
+    <t>Croation</t>
+  </si>
+  <si>
+    <t>Czech</t>
+  </si>
+  <si>
+    <t>Danish</t>
+  </si>
+  <si>
+    <t>Dutch</t>
+  </si>
+  <si>
+    <t>Finnish</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Greek</t>
+  </si>
+  <si>
+    <t>Hausa</t>
+  </si>
+  <si>
+    <t>Hindi</t>
+  </si>
+  <si>
+    <t>Indonesian</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>Japanese</t>
+  </si>
+  <si>
+    <t>Korean</t>
+  </si>
+  <si>
+    <t>Māori</t>
+  </si>
+  <si>
+    <t>Nepali</t>
+  </si>
+  <si>
+    <t>Persian</t>
+  </si>
+  <si>
+    <t>Portuguese - Brazil</t>
+  </si>
+  <si>
+    <t>Portuguese - Portugal</t>
+  </si>
+  <si>
+    <t>Spanish - Mexico</t>
+  </si>
+  <si>
+    <t>Spanish - Spain</t>
+  </si>
+  <si>
+    <t>Tamil</t>
+  </si>
+  <si>
+    <t>Thai</t>
+  </si>
+  <si>
+    <t>Ukrainian</t>
+  </si>
+  <si>
+    <t>Vietnamese</t>
+  </si>
+  <si>
+    <t>If your language is not listed, we may be able to collaborate on developing a validated translation.</t>
+  </si>
+  <si>
     <t>Option</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Global Observatory of Healthy and Sustainable Cities</t>
-  </si>
-  <si>
-    <t>Version 0.01</t>
-  </si>
-  <si>
-    <t>21 June 2024</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Summary</t>
-  </si>
-  <si>
-    <t>After reviewing the results, update this summary text to contextualise your findings, and relate to external text and documents (e.g. using website hyperlinks).  This text will be used in the report summary.</t>
-  </si>
-  <si>
-    <t>City context</t>
-  </si>
-  <si>
-    <t>Please briefly summarise the city location, history and topography, as relevant.</t>
-  </si>
-  <si>
-    <t>Demographics and health equity</t>
-  </si>
-  <si>
-    <t>Please highlight socio-economic demographic characteristics and key health challenges and inequities present in this urban area.</t>
-  </si>
-  <si>
-    <t>Environmental disaster context:</t>
-  </si>
-  <si>
-    <t>Completed policy checklist values will be added, but prose may be customised here to detail  environmental hazards likely to be experience by the urban area over the next 5-10 years</t>
-  </si>
-  <si>
-    <t>Country name, for example: سلطنة عُمان</t>
-  </si>
-  <si>
-    <t>City name, for example: مَسْقَط</t>
-  </si>
-  <si>
-    <t>Levels of Government</t>
-  </si>
-  <si>
-    <t>Completed policy checklist values will be added, but prose may be customised here to detail levels of government reviewed in the policy checklist using the appropriate terms for your study region.</t>
-  </si>
-  <si>
     <t>Response</t>
   </si>
   <si>
@@ -132,6 +228,9 @@
     <t>Image 3 file</t>
   </si>
   <si>
+    <t>Write filename for .jpg image 1000px by 1000px; or equivalent 1:1 aspect ratio. Please provide this file to the person generating the report.</t>
+  </si>
+  <si>
     <t>Image 3 credit</t>
   </si>
   <si>
@@ -139,112 +238,13 @@
   </si>
   <si>
     <t>Image 4 credit</t>
-  </si>
-  <si>
-    <t>Write filename for .jpg image 1000px by 1000px; or equivalent 1:1 aspect ratio. Please provide this file to the person generating the report.</t>
-  </si>
-  <si>
-    <t>Additional language* (rename this cell)</t>
-  </si>
-  <si>
-    <t>Arabic</t>
-  </si>
-  <si>
-    <t>Catalan</t>
-  </si>
-  <si>
-    <t>Chinese - Simplified</t>
-  </si>
-  <si>
-    <t>Chinese - Traditional</t>
-  </si>
-  <si>
-    <t>Croation</t>
-  </si>
-  <si>
-    <t>Czech</t>
-  </si>
-  <si>
-    <t>Danish</t>
-  </si>
-  <si>
-    <t>Dutch</t>
-  </si>
-  <si>
-    <t>Finnish</t>
-  </si>
-  <si>
-    <t>French</t>
-  </si>
-  <si>
-    <t>German</t>
-  </si>
-  <si>
-    <t>Greek</t>
-  </si>
-  <si>
-    <t>Hausa</t>
-  </si>
-  <si>
-    <t>Hindi</t>
-  </si>
-  <si>
-    <t>Indonesian</t>
-  </si>
-  <si>
-    <t>Italian</t>
-  </si>
-  <si>
-    <t>Japanese</t>
-  </si>
-  <si>
-    <t>Korean</t>
-  </si>
-  <si>
-    <t>Māori</t>
-  </si>
-  <si>
-    <t>Nepali</t>
-  </si>
-  <si>
-    <t>Persian</t>
-  </si>
-  <si>
-    <t>Portuguese - Brazil</t>
-  </si>
-  <si>
-    <t>Portuguese - Portugal</t>
-  </si>
-  <si>
-    <t>Spanish - Mexico</t>
-  </si>
-  <si>
-    <t>Spanish - Spain</t>
-  </si>
-  <si>
-    <t>Tamil</t>
-  </si>
-  <si>
-    <t>Thai</t>
-  </si>
-  <si>
-    <t>Ukrainian</t>
-  </si>
-  <si>
-    <t>Vietnamese</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Pending validation, additional language options may include: </t>
-  </si>
-  <si>
-    <t>If your language is not listed, we may be able to collaborate on developing a validated translation.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,7 +261,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,6 +280,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -421,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -433,22 +439,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -459,21 +456,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -529,8 +511,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -868,25 +871,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754352EF-86BE-49E3-B33E-435FA8A2B626}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.42578125" customWidth="1"/>
     <col min="2" max="2" width="54.7109375" style="2" customWidth="1"/>
     <col min="3" max="8" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="3"/>
+    <row r="1" spans="1:8">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -894,11 +897,11 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3"/>
+    <row r="2" spans="1:8">
+      <c r="A2" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="29"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -906,11 +909,11 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3"/>
+    <row r="3" spans="1:8">
+      <c r="A3" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="29"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -918,11 +921,11 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5"/>
+    <row r="4" spans="1:8">
+      <c r="A4" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="30"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -930,301 +933,301 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="17" t="str">
+    <row r="5" spans="1:8" ht="45" customHeight="1">
+      <c r="A5" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="28" t="str">
         <f>"Languages"&amp;CHAR(10)&amp;"(add new languages in columns to the right as required)"&amp;CHAR(10)&amp;"Please write over the example entries with your response"</f>
         <v>Languages
 (add new languages in columns to the right as required)
 Please write over the example entries with your response</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="20" t="s">
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="27"/>
+      <c r="B6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+    </row>
+    <row r="9" spans="1:8" ht="60">
+      <c r="A9" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+    </row>
+    <row r="10" spans="1:8" ht="29.25">
+      <c r="A10" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+    </row>
+    <row r="11" spans="1:8" ht="45">
+      <c r="A11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+    </row>
+    <row r="12" spans="1:8" ht="60">
+      <c r="A12" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+    </row>
+    <row r="13" spans="1:8" ht="60">
+      <c r="A13" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="24"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-    </row>
-    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-    </row>
-    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-    </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-    </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="47" spans="1:1">
+      <c r="A47" s="1" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1247,94 +1250,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E70F4B6-C0B4-4830-BE38-913C81CCB835}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="79.85546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="79.85546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>27</v>
+    <row r="1" spans="1:2">
+      <c r="A1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30">
+      <c r="A3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30">
+      <c r="A4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30">
+      <c r="A5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30">
+      <c r="A6" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30">
+      <c r="A7" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30">
+      <c r="A8" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30">
+      <c r="A9" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30">
+      <c r="A10" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added in updated reporting and region configuration file to templates
</commit_message>
<xml_diff>
--- a/process/configuration/templates/generate_policy_report_options.xlsx
+++ b/process/configuration/templates/generate_policy_report_options.xlsx
@@ -1346,4 +1346,10 @@
     <oddHeader>&amp;C&amp;"Calibri"&amp;12&amp;KEEDC00 RMIT Classification: Trusted&amp;1#_x000D_</oddHeader>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{8c3d088b-6243-4963-a2e2-8b321ab7f8fc}" enabled="1" method="Standard" siteId="{d1323671-cdbe-4417-b4d4-bdb24b51316b}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>